<commit_message>
add project accession to eva-schema
</commit_message>
<xml_diff>
--- a/tests/resources/EVA_Submission_Docker_Test.xlsx
+++ b/tests/resources/EVA_Submission_Docker_Test.xlsx
@@ -30,12 +30,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="558">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="566">
   <si>
     <t xml:space="preserve">PLEASE READ FIRST</t>
   </si>
   <si>
-    <t xml:space="preserve">V2.0.1 May 2025</t>
+    <t xml:space="preserve">V2.0.2 Sep 2025</t>
   </si>
   <si>
     <t xml:space="preserve">This Spreadsheet is meant to be used with the EVA submissions command line tools eva-sub-cli.</t>
@@ -90,7 +90,7 @@
     <t xml:space="preserve">Project</t>
   </si>
   <si>
-    <t xml:space="preserve">The objective of this sheet is to gather general information about the Project including submitter, submitting centre, collaborators and publications.</t>
+    <t xml:space="preserve">The objective of this sheet is to gather general information about the Project including submitter, submitting centre, collaborators and publications, if its a new project. In case of an existing project, you can just provide the project accession.</t>
   </si>
   <si>
     <t xml:space="preserve">Sample</t>
@@ -287,6 +287,21 @@
     <t xml:space="preserve">Data Expected</t>
   </si>
   <si>
+    <t xml:space="preserve">ATTENTION: Please complete EITHER Section 1: "Pre-existing project" OR Section 2: "New Project"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Section 1: "Pre-existing project"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project Accession</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accession of the project in case it already exists</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Section 2: "New Project"</t>
+  </si>
+  <si>
     <t xml:space="preserve">Project Title</t>
   </si>
   <si>
@@ -354,6 +369,38 @@
   </si>
   <si>
     <t xml:space="preserve">Brokering institution, if the submission is brokered by another institution to the center producing the project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pre-existing Project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Project</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">                                                                                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Project Basic Details</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">test_project_title</t>
@@ -813,9 +860,6 @@
   </si>
   <si>
     <t xml:space="preserve">Pre-registered sample(s)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OR</t>
   </si>
   <si>
     <t xml:space="preserve">Novel sample(s)</t>
@@ -2012,7 +2056,48 @@
       <charset val="1"/>
     </font>
     <font>
+      <i val="true"/>
+      <sz val="18"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <i val="true"/>
+      <u val="single"/>
+      <sz val="18"/>
+      <color rgb="FF008000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="12"/>
+      <color rgb="FF008000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -2045,27 +2130,9 @@
     </font>
     <font>
       <i val="true"/>
-      <sz val="18"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <i val="true"/>
       <u val="single"/>
       <sz val="18"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <i val="true"/>
-      <u val="single"/>
-      <sz val="18"/>
-      <color rgb="FF008000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -2086,33 +2153,10 @@
       <charset val="1"/>
     </font>
     <font>
-      <u val="single"/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <i val="true"/>
       <u val="single"/>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="20"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="12"/>
-      <color rgb="FF008000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -2305,7 +2349,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="84">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2334,7 +2378,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2438,15 +2482,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2454,11 +2506,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2470,35 +2538,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2506,15 +2550,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2526,11 +2582,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2566,11 +2618,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="20" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="2" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="20" fillId="2" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2578,7 +2630,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="2" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="25" fillId="2" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2610,7 +2662,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="20" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2622,7 +2674,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2886,10 +2938,10 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="61.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="83.5"/>
@@ -2954,7 +3006,7 @@
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" s="4" customFormat="true" ht="79.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" s="4" customFormat="true" ht="67.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="12" t="s">
         <v>4</v>
       </c>
@@ -2988,7 +3040,7 @@
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" s="4" customFormat="true" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" s="4" customFormat="true" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="15" t="s">
         <v>6</v>
       </c>
@@ -3016,7 +3068,7 @@
       </c>
       <c r="B11" s="16"/>
     </row>
-    <row r="12" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="17" t="s">
         <v>8</v>
       </c>
@@ -3024,7 +3076,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="19" t="s">
         <v>10</v>
       </c>
@@ -3033,7 +3085,7 @@
       </c>
       <c r="C13" s="21"/>
     </row>
-    <row r="14" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="50.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="22" t="s">
         <v>12</v>
       </c>
@@ -3041,7 +3093,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="79.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="67.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="23" t="s">
         <v>14</v>
       </c>
@@ -3049,7 +3101,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="98.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="83.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="24" t="s">
         <v>16</v>
       </c>
@@ -3057,7 +3109,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="59.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="50.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="25" t="s">
         <v>18</v>
       </c>
@@ -3131,7 +3183,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33.33"/>
@@ -3139,18 +3191,18 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="28" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="31" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6182,7 +6234,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="39"/>
@@ -6190,1655 +6242,1655 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="25"/>
   </cols>
   <sheetData>
-    <row r="1" s="50" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="79" t="s">
-        <v>206</v>
-      </c>
-      <c r="D1" s="79" t="s">
+    <row r="1" s="53" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="81" t="s">
+        <v>214</v>
+      </c>
+      <c r="D1" s="81" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="33" t="s">
-        <v>127</v>
-      </c>
-      <c r="B2" s="33" t="s">
-        <v>154</v>
-      </c>
-      <c r="D2" s="33" t="s">
-        <v>68</v>
-      </c>
-      <c r="E2" s="33" t="s">
-        <v>74</v>
+      <c r="A2" s="35" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>163</v>
+      </c>
+      <c r="D2" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" s="35" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="F3" s="80"/>
+        <v>217</v>
+      </c>
+      <c r="F3" s="82"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>210</v>
+        <v>218</v>
       </c>
       <c r="B4" s="31" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="B7" s="31" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>225</v>
+        <v>233</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>226</v>
+        <v>234</v>
       </c>
       <c r="B8" s="31" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>228</v>
+        <v>236</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>229</v>
+        <v>237</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>232</v>
+        <v>240</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>233</v>
+        <v>241</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>234</v>
+        <v>242</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>235</v>
+        <v>243</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>236</v>
+        <v>244</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>237</v>
+        <v>245</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>238</v>
+        <v>246</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>239</v>
+        <v>247</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>240</v>
+        <v>248</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>242</v>
+        <v>250</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>240</v>
+        <v>248</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="31" t="s">
-        <v>243</v>
+        <v>251</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="31" t="s">
-        <v>245</v>
+        <v>253</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>246</v>
+        <v>254</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="31" t="s">
-        <v>247</v>
+        <v>255</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>248</v>
+        <v>256</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="31" t="s">
-        <v>249</v>
+        <v>257</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>250</v>
+        <v>258</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="31" t="s">
-        <v>251</v>
+        <v>259</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>252</v>
+        <v>260</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="31" t="s">
-        <v>253</v>
+        <v>261</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>254</v>
+        <v>262</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="31" t="s">
-        <v>255</v>
+        <v>263</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>256</v>
+        <v>264</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="31" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>258</v>
+        <v>266</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="31" t="s">
-        <v>259</v>
+        <v>267</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>260</v>
+        <v>268</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="31" t="s">
-        <v>261</v>
+        <v>269</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>262</v>
+        <v>270</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="31" t="s">
-        <v>263</v>
+        <v>271</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>264</v>
+        <v>272</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="31" t="s">
-        <v>265</v>
+        <v>273</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>266</v>
+        <v>274</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="31" t="s">
-        <v>267</v>
+        <v>275</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>268</v>
+        <v>276</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="31" t="s">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>270</v>
+        <v>278</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="31" t="s">
-        <v>271</v>
+        <v>279</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="31" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>274</v>
+        <v>282</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="31" t="s">
-        <v>275</v>
+        <v>283</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>276</v>
+        <v>284</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="31" t="s">
-        <v>277</v>
+        <v>285</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="31" t="s">
-        <v>279</v>
+        <v>287</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>280</v>
+        <v>288</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="31" t="s">
-        <v>281</v>
+        <v>289</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>282</v>
+        <v>290</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="31" t="s">
-        <v>283</v>
+        <v>291</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>284</v>
+        <v>292</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="31" t="s">
-        <v>285</v>
+        <v>293</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>286</v>
+        <v>294</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="31" t="s">
-        <v>287</v>
+        <v>295</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>288</v>
+        <v>296</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="31" t="s">
-        <v>289</v>
+        <v>297</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>290</v>
+        <v>298</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="31" t="s">
-        <v>291</v>
+        <v>299</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>292</v>
+        <v>300</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="31" t="s">
-        <v>293</v>
+        <v>301</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>294</v>
+        <v>302</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="31" t="s">
-        <v>295</v>
+        <v>303</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>296</v>
+        <v>304</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="31" t="s">
-        <v>297</v>
+        <v>305</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>298</v>
+        <v>306</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="31" t="s">
-        <v>299</v>
+        <v>307</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>300</v>
+        <v>308</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="31" t="s">
-        <v>301</v>
+        <v>309</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>302</v>
+        <v>310</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="31" t="s">
-        <v>303</v>
+        <v>311</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>304</v>
+        <v>312</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="31" t="s">
-        <v>305</v>
+        <v>313</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>306</v>
+        <v>314</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="31" t="s">
-        <v>307</v>
+        <v>315</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>308</v>
+        <v>316</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="31" t="s">
-        <v>309</v>
+        <v>317</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>310</v>
+        <v>318</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="31" t="s">
-        <v>311</v>
+        <v>319</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>312</v>
+        <v>320</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="31" t="s">
-        <v>313</v>
+        <v>321</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>314</v>
+        <v>322</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="31" t="s">
-        <v>315</v>
+        <v>323</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>316</v>
+        <v>324</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="31" t="s">
-        <v>317</v>
+        <v>325</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>318</v>
+        <v>326</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="31" t="s">
-        <v>319</v>
+        <v>327</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>320</v>
+        <v>328</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="31" t="s">
-        <v>321</v>
+        <v>329</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>322</v>
+        <v>330</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="31" t="s">
-        <v>323</v>
+        <v>331</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>324</v>
+        <v>332</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="31" t="s">
-        <v>325</v>
+        <v>333</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="31" t="s">
-        <v>326</v>
-      </c>
-      <c r="E55" s="50"/>
+        <v>334</v>
+      </c>
+      <c r="E55" s="53"/>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="31" t="s">
-        <v>327</v>
+        <v>335</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="31" t="s">
-        <v>328</v>
+        <v>336</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="31" t="s">
-        <v>329</v>
+        <v>337</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="31" t="s">
-        <v>330</v>
+        <v>338</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="31" t="s">
-        <v>331</v>
+        <v>339</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="31" t="s">
-        <v>332</v>
+        <v>340</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="31" t="s">
-        <v>333</v>
+        <v>341</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="31" t="s">
-        <v>334</v>
+        <v>342</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="31" t="s">
-        <v>335</v>
+        <v>343</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="31" t="s">
-        <v>336</v>
+        <v>344</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="31" t="s">
-        <v>337</v>
+        <v>345</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="31" t="s">
-        <v>338</v>
+        <v>346</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="31" t="s">
-        <v>339</v>
+        <v>347</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="31" t="s">
-        <v>340</v>
+        <v>348</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="31" t="s">
-        <v>341</v>
+        <v>349</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="31" t="s">
-        <v>342</v>
+        <v>350</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="31" t="s">
-        <v>343</v>
+        <v>351</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="31" t="s">
-        <v>344</v>
+        <v>352</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="31" t="s">
-        <v>345</v>
+        <v>353</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="31" t="s">
-        <v>346</v>
+        <v>354</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="31" t="s">
-        <v>347</v>
+        <v>355</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="31" t="s">
-        <v>348</v>
+        <v>356</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="31" t="s">
-        <v>349</v>
+        <v>357</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="31" t="s">
-        <v>350</v>
+        <v>358</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="31" t="s">
-        <v>351</v>
+        <v>359</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="31" t="s">
-        <v>352</v>
+        <v>360</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="31" t="s">
-        <v>353</v>
+        <v>361</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="31" t="s">
-        <v>354</v>
+        <v>362</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="31" t="s">
-        <v>355</v>
+        <v>363</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B85" s="31" t="s">
-        <v>356</v>
+        <v>364</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B86" s="31" t="s">
-        <v>357</v>
+        <v>365</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="31" t="s">
-        <v>358</v>
+        <v>366</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="31" t="s">
-        <v>359</v>
+        <v>367</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B89" s="31" t="s">
-        <v>360</v>
+        <v>368</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B90" s="31" t="s">
-        <v>361</v>
+        <v>369</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B91" s="31" t="s">
-        <v>362</v>
+        <v>370</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B92" s="31" t="s">
-        <v>363</v>
+        <v>371</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B93" s="31" t="s">
-        <v>364</v>
+        <v>372</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B94" s="31" t="s">
-        <v>365</v>
+        <v>373</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B95" s="31" t="s">
-        <v>366</v>
+        <v>374</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B96" s="31" t="s">
-        <v>367</v>
+        <v>375</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B97" s="31" t="s">
-        <v>368</v>
+        <v>376</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B98" s="31" t="s">
-        <v>369</v>
+        <v>377</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B99" s="31" t="s">
-        <v>370</v>
+        <v>378</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B100" s="31" t="s">
-        <v>371</v>
+        <v>379</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B101" s="31" t="s">
-        <v>372</v>
+        <v>380</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B102" s="31" t="s">
-        <v>373</v>
+        <v>381</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B103" s="31" t="s">
-        <v>374</v>
+        <v>382</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B104" s="31" t="s">
-        <v>375</v>
+        <v>383</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B105" s="31" t="s">
-        <v>376</v>
+        <v>384</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B106" s="31" t="s">
-        <v>377</v>
+        <v>385</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B107" s="31" t="s">
-        <v>378</v>
+        <v>386</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B108" s="31" t="s">
-        <v>379</v>
+        <v>387</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B109" s="31" t="s">
-        <v>380</v>
+        <v>388</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B110" s="31" t="s">
-        <v>381</v>
+        <v>389</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B111" s="31" t="s">
-        <v>382</v>
+        <v>390</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B112" s="31" t="s">
-        <v>383</v>
+        <v>391</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B113" s="31" t="s">
-        <v>384</v>
+        <v>392</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B114" s="31" t="s">
-        <v>385</v>
+        <v>393</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B115" s="31" t="s">
-        <v>386</v>
+        <v>394</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B116" s="31" t="s">
-        <v>387</v>
+        <v>395</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B117" s="31" t="s">
-        <v>388</v>
+        <v>396</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B118" s="31" t="s">
-        <v>389</v>
+        <v>397</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B119" s="31" t="s">
-        <v>390</v>
+        <v>398</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B120" s="31" t="s">
-        <v>391</v>
+        <v>399</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B121" s="31" t="s">
-        <v>392</v>
+        <v>400</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B122" s="31" t="s">
-        <v>393</v>
+        <v>401</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B123" s="31" t="s">
-        <v>394</v>
+        <v>402</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B124" s="31" t="s">
-        <v>395</v>
+        <v>403</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B125" s="31" t="s">
-        <v>396</v>
+        <v>404</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B126" s="31" t="s">
-        <v>397</v>
+        <v>405</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B127" s="31" t="s">
-        <v>398</v>
+        <v>406</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B128" s="31" t="s">
-        <v>399</v>
+        <v>407</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B129" s="31" t="s">
-        <v>400</v>
+        <v>408</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B130" s="31" t="s">
-        <v>401</v>
+        <v>409</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B131" s="31" t="s">
-        <v>402</v>
+        <v>410</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B132" s="31" t="s">
-        <v>403</v>
+        <v>411</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B133" s="31" t="s">
-        <v>404</v>
+        <v>412</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B134" s="31" t="s">
-        <v>405</v>
+        <v>413</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B135" s="31" t="s">
-        <v>406</v>
+        <v>414</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B136" s="31" t="s">
-        <v>407</v>
+        <v>415</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B137" s="31" t="s">
-        <v>408</v>
+        <v>416</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B138" s="31" t="s">
-        <v>409</v>
+        <v>417</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B139" s="31" t="s">
-        <v>410</v>
+        <v>418</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B140" s="31" t="s">
-        <v>411</v>
+        <v>419</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B141" s="31" t="s">
-        <v>412</v>
+        <v>420</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B142" s="31" t="s">
-        <v>413</v>
+        <v>421</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B143" s="31" t="s">
-        <v>414</v>
+        <v>422</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B144" s="31" t="s">
-        <v>415</v>
+        <v>423</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B145" s="31" t="s">
-        <v>416</v>
+        <v>424</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B146" s="31" t="s">
-        <v>417</v>
+        <v>425</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B147" s="31" t="s">
-        <v>418</v>
+        <v>426</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B148" s="31" t="s">
-        <v>419</v>
+        <v>427</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B149" s="31" t="s">
-        <v>420</v>
+        <v>428</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B150" s="31" t="s">
-        <v>421</v>
+        <v>429</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B151" s="31" t="s">
-        <v>422</v>
+        <v>430</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B152" s="31" t="s">
-        <v>423</v>
+        <v>431</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B153" s="31" t="s">
-        <v>424</v>
+        <v>432</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B154" s="31" t="s">
-        <v>425</v>
+        <v>433</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B155" s="31" t="s">
-        <v>426</v>
+        <v>434</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B156" s="31" t="s">
-        <v>427</v>
+        <v>435</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B157" s="31" t="s">
-        <v>428</v>
+        <v>436</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B158" s="31" t="s">
-        <v>429</v>
+        <v>437</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B159" s="31" t="s">
-        <v>430</v>
+        <v>438</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B160" s="31" t="s">
-        <v>431</v>
+        <v>439</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B161" s="31" t="s">
-        <v>432</v>
+        <v>440</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B162" s="31" t="s">
-        <v>433</v>
+        <v>441</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B163" s="31" t="s">
-        <v>434</v>
+        <v>442</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B164" s="31" t="s">
-        <v>435</v>
+        <v>443</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B165" s="31" t="s">
-        <v>436</v>
+        <v>444</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B166" s="31" t="s">
-        <v>437</v>
+        <v>445</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B167" s="31" t="s">
-        <v>438</v>
+        <v>446</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B168" s="31" t="s">
-        <v>439</v>
+        <v>447</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B169" s="31" t="s">
-        <v>440</v>
+        <v>448</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B170" s="31" t="s">
-        <v>441</v>
+        <v>449</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B171" s="31" t="s">
-        <v>442</v>
+        <v>450</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B172" s="31" t="s">
-        <v>443</v>
+        <v>451</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B173" s="31" t="s">
-        <v>444</v>
+        <v>452</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B174" s="31" t="s">
-        <v>445</v>
+        <v>453</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B175" s="31" t="s">
-        <v>446</v>
+        <v>454</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B176" s="31" t="s">
-        <v>447</v>
+        <v>455</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B177" s="31" t="s">
-        <v>448</v>
+        <v>456</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B178" s="31" t="s">
-        <v>449</v>
+        <v>457</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B179" s="31" t="s">
-        <v>450</v>
+        <v>458</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B180" s="31" t="s">
-        <v>451</v>
+        <v>459</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B181" s="31" t="s">
-        <v>452</v>
+        <v>460</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B182" s="31" t="s">
-        <v>453</v>
+        <v>461</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B183" s="31" t="s">
-        <v>454</v>
+        <v>462</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B184" s="31" t="s">
-        <v>455</v>
+        <v>463</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B185" s="31" t="s">
-        <v>456</v>
+        <v>464</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B186" s="31" t="s">
-        <v>457</v>
+        <v>465</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B187" s="31" t="s">
-        <v>458</v>
+        <v>466</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B188" s="31" t="s">
-        <v>459</v>
+        <v>467</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B189" s="31" t="s">
-        <v>460</v>
+        <v>468</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B190" s="31" t="s">
-        <v>461</v>
+        <v>469</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B191" s="31" t="s">
-        <v>462</v>
+        <v>470</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B192" s="31" t="s">
-        <v>463</v>
+        <v>471</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B193" s="31" t="s">
-        <v>464</v>
+        <v>472</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B194" s="31" t="s">
-        <v>465</v>
+        <v>473</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B195" s="31" t="s">
-        <v>466</v>
+        <v>474</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B196" s="31" t="s">
-        <v>467</v>
+        <v>475</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B197" s="31" t="s">
-        <v>468</v>
+        <v>476</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B198" s="31" t="s">
-        <v>469</v>
+        <v>477</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B199" s="31" t="s">
-        <v>470</v>
+        <v>478</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B200" s="31" t="s">
-        <v>471</v>
+        <v>479</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B201" s="31" t="s">
-        <v>472</v>
+        <v>480</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B202" s="31" t="s">
-        <v>473</v>
+        <v>481</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B203" s="31" t="s">
-        <v>474</v>
+        <v>482</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B204" s="31" t="s">
-        <v>475</v>
+        <v>483</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B205" s="31" t="s">
-        <v>476</v>
+        <v>484</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B206" s="31" t="s">
-        <v>477</v>
+        <v>485</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B207" s="31" t="s">
-        <v>478</v>
+        <v>486</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B208" s="31" t="s">
-        <v>479</v>
+        <v>487</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B209" s="31" t="s">
-        <v>480</v>
+        <v>488</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B210" s="31" t="s">
-        <v>481</v>
+        <v>489</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B211" s="31" t="s">
-        <v>482</v>
+        <v>490</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B212" s="31" t="s">
-        <v>483</v>
+        <v>491</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B213" s="31" t="s">
-        <v>484</v>
+        <v>492</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B214" s="31" t="s">
-        <v>485</v>
+        <v>493</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B215" s="31" t="s">
-        <v>486</v>
+        <v>494</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B216" s="31" t="s">
-        <v>487</v>
+        <v>495</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B217" s="31" t="s">
-        <v>488</v>
+        <v>496</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B218" s="31" t="s">
-        <v>489</v>
+        <v>497</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B219" s="31" t="s">
-        <v>490</v>
+        <v>498</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B220" s="31" t="s">
-        <v>491</v>
+        <v>499</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B221" s="31" t="s">
-        <v>492</v>
+        <v>500</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B222" s="31" t="s">
-        <v>493</v>
+        <v>501</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B223" s="31" t="s">
-        <v>494</v>
+        <v>502</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B224" s="31" t="s">
-        <v>495</v>
+        <v>503</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B225" s="31" t="s">
-        <v>496</v>
+        <v>504</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B226" s="31" t="s">
-        <v>497</v>
+        <v>505</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B227" s="31" t="s">
-        <v>498</v>
+        <v>506</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B228" s="31" t="s">
-        <v>499</v>
+        <v>507</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B229" s="31" t="s">
-        <v>500</v>
+        <v>508</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B230" s="31" t="s">
-        <v>501</v>
+        <v>509</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B231" s="31" t="s">
-        <v>502</v>
+        <v>510</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B232" s="31" t="s">
-        <v>503</v>
+        <v>511</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B233" s="31" t="s">
-        <v>504</v>
+        <v>512</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B234" s="31" t="s">
-        <v>505</v>
+        <v>513</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B235" s="31" t="s">
-        <v>506</v>
+        <v>514</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B236" s="31" t="s">
-        <v>507</v>
+        <v>515</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B237" s="31" t="s">
-        <v>508</v>
+        <v>516</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B238" s="31" t="s">
-        <v>509</v>
+        <v>517</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B239" s="31" t="s">
-        <v>510</v>
+        <v>518</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B240" s="31" t="s">
-        <v>511</v>
+        <v>519</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B241" s="31" t="s">
-        <v>512</v>
+        <v>520</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B242" s="31" t="s">
-        <v>513</v>
+        <v>521</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B243" s="31" t="s">
-        <v>514</v>
+        <v>522</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B244" s="31" t="s">
-        <v>515</v>
+        <v>523</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B245" s="31" t="s">
-        <v>516</v>
+        <v>524</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B246" s="31" t="s">
-        <v>517</v>
+        <v>525</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B247" s="31" t="s">
-        <v>518</v>
+        <v>526</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B248" s="31" t="s">
-        <v>519</v>
+        <v>527</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B249" s="31" t="s">
-        <v>520</v>
+        <v>528</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B250" s="31" t="s">
-        <v>521</v>
+        <v>529</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B251" s="31" t="s">
-        <v>522</v>
+        <v>530</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B252" s="31" t="s">
-        <v>523</v>
+        <v>531</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B253" s="31" t="s">
-        <v>524</v>
+        <v>532</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B254" s="31" t="s">
-        <v>525</v>
+        <v>533</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B255" s="31" t="s">
-        <v>526</v>
+        <v>534</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B256" s="31" t="s">
-        <v>527</v>
+        <v>535</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B257" s="31" t="s">
-        <v>528</v>
+        <v>536</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B258" s="31" t="s">
-        <v>529</v>
+        <v>537</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B259" s="31" t="s">
-        <v>530</v>
+        <v>538</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B260" s="31" t="s">
-        <v>531</v>
+        <v>539</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B261" s="31" t="s">
-        <v>532</v>
+        <v>540</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B262" s="31" t="s">
-        <v>533</v>
+        <v>541</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B263" s="31" t="s">
-        <v>534</v>
+        <v>542</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B264" s="31" t="s">
-        <v>535</v>
+        <v>543</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B265" s="31" t="s">
-        <v>536</v>
+        <v>544</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B266" s="31" t="s">
-        <v>537</v>
+        <v>545</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B267" s="31" t="s">
-        <v>538</v>
+        <v>546</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B268" s="31" t="s">
-        <v>539</v>
+        <v>547</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B269" s="31" t="s">
-        <v>540</v>
+        <v>548</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B270" s="31" t="s">
-        <v>541</v>
+        <v>549</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B271" s="31" t="s">
-        <v>542</v>
+        <v>550</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B272" s="31" t="s">
-        <v>543</v>
+        <v>551</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B273" s="31" t="s">
-        <v>544</v>
+        <v>552</v>
       </c>
     </row>
     <row r="274" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B274" s="31" t="s">
-        <v>545</v>
+        <v>553</v>
       </c>
     </row>
     <row r="275" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B275" s="31" t="s">
-        <v>546</v>
+        <v>554</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B276" s="31" t="s">
-        <v>547</v>
+        <v>555</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B277" s="31" t="s">
-        <v>548</v>
+        <v>556</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B278" s="31" t="s">
-        <v>549</v>
+        <v>557</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B279" s="31" t="s">
-        <v>550</v>
+        <v>558</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B280" s="31" t="s">
-        <v>551</v>
+        <v>559</v>
       </c>
     </row>
     <row r="281" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B281" s="31" t="s">
-        <v>552</v>
+        <v>560</v>
       </c>
     </row>
     <row r="282" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B282" s="31" t="s">
-        <v>553</v>
+        <v>561</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B283" s="81" t="s">
-        <v>554</v>
+      <c r="B283" s="83" t="s">
+        <v>562</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B284" s="81" t="s">
-        <v>555</v>
+      <c r="B284" s="83" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B285" s="81" t="s">
-        <v>556</v>
+      <c r="B285" s="83" t="s">
+        <v>564</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B286" s="81" t="s">
-        <v>557</v>
+      <c r="B286" s="83" t="s">
+        <v>565</v>
       </c>
     </row>
   </sheetData>
@@ -7864,7 +7916,7 @@
       <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.33"/>
@@ -7927,13 +7979,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="176.66"/>
@@ -7947,100 +7999,123 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="57" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="1" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="42" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="34" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="33" t="s">
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="34" t="s">
+    <row r="5" customFormat="false" ht="42" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="36" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="35" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="B8" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="B7" s="1" t="s">
+    </row>
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="35" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B12" s="1" t="s">
+    </row>
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="35" t="s">
+      <c r="B14" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="35" t="s">
+    </row>
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
         <v>59</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" s="37" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -8060,84 +8135,147 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.3671875" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="54.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="6.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="34.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="14.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="40.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="36" width="16.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="64.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="1" width="6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="6.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="5.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="20.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="12.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="13.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="38" width="13.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="6.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="9.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="13.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="6.59"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1" s="28" t="s">
+      <c r="A1" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+    </row>
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="28"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="42" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="42"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+    </row>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="B3" s="40"/>
+      <c r="C3" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="E1" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="F1" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="G1" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="H1" s="30" t="s">
-        <v>50</v>
-      </c>
-      <c r="I1" s="30" t="s">
-        <v>52</v>
-      </c>
-      <c r="J1" s="37" t="s">
-        <v>54</v>
-      </c>
-      <c r="K1" s="30" t="s">
-        <v>56</v>
-      </c>
-      <c r="L1" s="38" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="31" t="s">
-        <v>60</v>
-      </c>
-      <c r="B2" s="31" t="s">
+      <c r="F3" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="H3" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="I3" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="J3" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="K3" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="L3" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="M3" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="D2" s="1" t="n">
+      <c r="N3" s="44" t="s">
+        <v>63</v>
+      </c>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+    </row>
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C4" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="E4" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="F4" s="1" t="n">
         <v>1234</v>
       </c>
+      <c r="J4" s="1"/>
+      <c r="L4" s="38"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="On which date can the data be released publicly. In the format yyyy-mm-dd" promptTitle="Private data" showDropDown="false" showErrorMessage="false" showInputMessage="true" sqref="J1:J1001" type="none">
+  <mergeCells count="2">
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C2:N2"/>
+  </mergeCells>
+  <dataValidations count="2">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="On which date can the data be released publicly. In the format yyyy-mm-dd" promptTitle="Private data" showDropDown="false" showErrorMessage="false" showInputMessage="true" sqref="L1:L4 J5:J1001" type="none">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="These sample names must match those provided in the VCF file(s)" promptTitle="Metadata and VCF" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B1" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -8163,7 +8301,7 @@
       <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="164.83"/>
@@ -8178,127 +8316,127 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="33" t="s">
-        <v>63</v>
+      <c r="A2" s="35" t="s">
+        <v>72</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="33" t="s">
-        <v>65</v>
+      <c r="A3" s="35" t="s">
+        <v>74</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="33" t="s">
-        <v>39</v>
+      <c r="A4" s="35" t="s">
+        <v>44</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="33" t="s">
-        <v>68</v>
+      <c r="A5" s="35" t="s">
+        <v>77</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="33" t="s">
-        <v>70</v>
+      <c r="A6" s="35" t="s">
+        <v>79</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="31" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>81</v>
+        <v>89</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>83</v>
+        <v>91</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="33"/>
+      <c r="A20" s="35"/>
     </row>
   </sheetData>
   <sheetProtection sheet="true" password="e50b" objects="true" scenarios="true"/>
@@ -8329,7 +8467,7 @@
       <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.51"/>
@@ -8348,72 +8486,72 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="28" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="C1" s="28" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="D1" s="28" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="E1" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="F1" s="39" t="s">
-        <v>72</v>
+        <v>79</v>
+      </c>
+      <c r="F1" s="45" t="s">
+        <v>81</v>
       </c>
       <c r="G1" s="30" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="H1" s="30" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="I1" s="30" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="J1" s="30" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="K1" s="30" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="L1" s="30" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="M1" s="30" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="N1" s="30" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="O1" s="30" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="31" t="s">
-        <v>91</v>
-      </c>
-      <c r="B2" s="35" t="s">
-        <v>92</v>
+        <v>100</v>
+      </c>
+      <c r="B2" s="37" t="s">
+        <v>101</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="E2" s="31" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="F2" s="31"/>
       <c r="G2" s="31"/>
       <c r="J2" s="31"/>
       <c r="K2" s="31"/>
-      <c r="M2" s="40"/>
+      <c r="M2" s="46"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D3" s="31"/>
@@ -8424,7 +8562,7 @@
       <c r="K3" s="31"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="35"/>
+      <c r="C4" s="37"/>
       <c r="D4" s="31"/>
       <c r="E4" s="31"/>
       <c r="F4" s="31"/>
@@ -16460,7 +16598,7 @@
       <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="44.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="215"/>
@@ -16475,440 +16613,440 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="42" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="41" t="s">
-        <v>96</v>
+      <c r="A2" s="47" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="42" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="42" t="s">
-        <v>97</v>
+      <c r="A3" s="48" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="33" t="s">
-        <v>65</v>
-      </c>
-      <c r="B4" s="43" t="s">
-        <v>98</v>
+      <c r="A4" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="49" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="34" t="s">
-        <v>99</v>
-      </c>
-      <c r="B5" s="43" t="s">
-        <v>100</v>
-      </c>
-      <c r="C5" s="34"/>
+      <c r="A5" s="50" t="s">
+        <v>108</v>
+      </c>
+      <c r="B5" s="49" t="s">
+        <v>109</v>
+      </c>
+      <c r="C5" s="50"/>
     </row>
     <row r="6" customFormat="false" ht="57" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="44" t="s">
-        <v>101</v>
+      <c r="A6" s="33" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="42" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="45" t="s">
-        <v>102</v>
+      <c r="A7" s="34" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="46" t="s">
-        <v>103</v>
-      </c>
-      <c r="B8" s="47" t="s">
-        <v>104</v>
+      <c r="A8" s="51" t="s">
+        <v>112</v>
+      </c>
+      <c r="B8" s="49" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="42" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="48" t="s">
-        <v>105</v>
+      <c r="A9" s="36" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="49" t="s">
-        <v>106</v>
+      <c r="A10" s="52" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="34" t="s">
-        <v>107</v>
-      </c>
-      <c r="B11" s="43" t="s">
-        <v>108</v>
+      <c r="A11" s="50" t="s">
+        <v>116</v>
+      </c>
+      <c r="B11" s="49" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="33" t="s">
-        <v>109</v>
-      </c>
-      <c r="B12" s="43" t="s">
-        <v>110</v>
+      <c r="A12" s="35" t="s">
+        <v>118</v>
+      </c>
+      <c r="B12" s="49" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" s="43" t="s">
-        <v>111</v>
+        <v>44</v>
+      </c>
+      <c r="B13" s="49" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B14" s="43" t="s">
-        <v>113</v>
+        <v>121</v>
+      </c>
+      <c r="B14" s="49" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B15" s="43" t="s">
-        <v>115</v>
+        <v>123</v>
+      </c>
+      <c r="B15" s="49" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B16" s="43" t="s">
-        <v>117</v>
+        <v>125</v>
+      </c>
+      <c r="B16" s="49" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="50" t="s">
-        <v>118</v>
-      </c>
-      <c r="B17" s="43"/>
-    </row>
-    <row r="18" customFormat="false" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="B18" s="51" t="s">
-        <v>119</v>
+      <c r="A17" s="53" t="s">
+        <v>127</v>
+      </c>
+      <c r="B17" s="49"/>
+    </row>
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="54" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="33" t="s">
-        <v>120</v>
-      </c>
-      <c r="B19" s="43" t="s">
-        <v>121</v>
+      <c r="A19" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="B19" s="49" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B20" s="43" t="s">
-        <v>123</v>
+        <v>131</v>
+      </c>
+      <c r="B20" s="49" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="50" t="s">
-        <v>124</v>
-      </c>
-      <c r="B21" s="43"/>
+      <c r="A21" s="53" t="s">
+        <v>133</v>
+      </c>
+      <c r="B21" s="49"/>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B22" s="43" t="s">
-        <v>126</v>
+        <v>134</v>
+      </c>
+      <c r="B22" s="49" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B23" s="43" t="s">
-        <v>128</v>
+        <v>136</v>
+      </c>
+      <c r="B23" s="49" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="B24" s="43" t="s">
-        <v>130</v>
+        <v>138</v>
+      </c>
+      <c r="B24" s="49" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="50" t="s">
-        <v>131</v>
-      </c>
-      <c r="B25" s="43"/>
+      <c r="A25" s="53" t="s">
+        <v>140</v>
+      </c>
+      <c r="B25" s="49"/>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="B26" s="43" t="s">
-        <v>133</v>
+        <v>141</v>
+      </c>
+      <c r="B26" s="49" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="B27" s="43" t="s">
-        <v>135</v>
+        <v>143</v>
+      </c>
+      <c r="B27" s="49" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="B28" s="43" t="s">
-        <v>137</v>
+        <v>145</v>
+      </c>
+      <c r="B28" s="49" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="B29" s="43" t="s">
-        <v>139</v>
+        <v>147</v>
+      </c>
+      <c r="B29" s="49" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B30" s="43" t="s">
-        <v>141</v>
+        <v>149</v>
+      </c>
+      <c r="B30" s="49" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="50" t="s">
-        <v>142</v>
-      </c>
-      <c r="B31" s="43"/>
+      <c r="A31" s="53" t="s">
+        <v>151</v>
+      </c>
+      <c r="B31" s="49"/>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="B32" s="43" t="s">
-        <v>144</v>
+        <v>152</v>
+      </c>
+      <c r="B32" s="49" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="B33" s="43" t="s">
-        <v>146</v>
+        <v>154</v>
+      </c>
+      <c r="B33" s="49" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="B34" s="43" t="s">
-        <v>148</v>
+        <v>156</v>
+      </c>
+      <c r="B34" s="49" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="50" t="s">
-        <v>149</v>
-      </c>
-      <c r="B35" s="43"/>
+      <c r="A35" s="53" t="s">
+        <v>158</v>
+      </c>
+      <c r="B35" s="49"/>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="B36" s="43" t="s">
-        <v>151</v>
+        <v>159</v>
+      </c>
+      <c r="B36" s="49" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="33" t="s">
-        <v>152</v>
-      </c>
-      <c r="B37" s="43" t="s">
-        <v>153</v>
+      <c r="A37" s="35" t="s">
+        <v>161</v>
+      </c>
+      <c r="B37" s="49" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="33" t="s">
-        <v>154</v>
-      </c>
-      <c r="B38" s="43" t="s">
-        <v>155</v>
+      <c r="A38" s="35" t="s">
+        <v>163</v>
+      </c>
+      <c r="B38" s="49" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="B39" s="43" t="s">
-        <v>157</v>
+        <v>165</v>
+      </c>
+      <c r="B39" s="49" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="B40" s="43" t="s">
-        <v>159</v>
+        <v>167</v>
+      </c>
+      <c r="B40" s="49" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="B41" s="43" t="s">
-        <v>161</v>
+        <v>169</v>
+      </c>
+      <c r="B41" s="49" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="B42" s="43" t="s">
-        <v>163</v>
+        <v>171</v>
+      </c>
+      <c r="B42" s="49" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="B43" s="43" t="s">
-        <v>165</v>
+        <v>173</v>
+      </c>
+      <c r="B43" s="49" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="B44" s="43" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="50.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>175</v>
+      </c>
+      <c r="B44" s="49" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B45" s="51" t="s">
-        <v>169</v>
+        <v>177</v>
+      </c>
+      <c r="B45" s="54" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="50" t="s">
-        <v>170</v>
-      </c>
-      <c r="B46" s="43"/>
+      <c r="A46" s="53" t="s">
+        <v>179</v>
+      </c>
+      <c r="B46" s="49"/>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="B47" s="43" t="s">
-        <v>172</v>
+        <v>180</v>
+      </c>
+      <c r="B47" s="49" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="B48" s="43" t="s">
-        <v>174</v>
+        <v>182</v>
+      </c>
+      <c r="B48" s="49" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="B49" s="43" t="s">
-        <v>176</v>
+        <v>184</v>
+      </c>
+      <c r="B49" s="49" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="B50" s="43" t="s">
-        <v>178</v>
+        <v>186</v>
+      </c>
+      <c r="B50" s="49" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="B51" s="43" t="s">
-        <v>180</v>
+        <v>188</v>
+      </c>
+      <c r="B51" s="49" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="B52" s="43" t="s">
-        <v>182</v>
+        <v>190</v>
+      </c>
+      <c r="B52" s="49" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="B53" s="43" t="s">
-        <v>184</v>
+        <v>192</v>
+      </c>
+      <c r="B53" s="49" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="B54" s="43" t="s">
-        <v>186</v>
+        <v>194</v>
+      </c>
+      <c r="B54" s="49" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="B55" s="43" t="s">
-        <v>188</v>
+        <v>196</v>
+      </c>
+      <c r="B55" s="49" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="B56" s="43" t="s">
-        <v>190</v>
+        <v>198</v>
+      </c>
+      <c r="B56" s="49" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="50" t="s">
-        <v>191</v>
-      </c>
-      <c r="B57" s="43"/>
+      <c r="A57" s="53" t="s">
+        <v>200</v>
+      </c>
+      <c r="B57" s="49"/>
     </row>
     <row r="58" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="41" t="s">
-        <v>192</v>
-      </c>
-      <c r="B58" s="43"/>
+      <c r="A58" s="47" t="s">
+        <v>201</v>
+      </c>
+      <c r="B58" s="49"/>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="52" t="s">
-        <v>193</v>
-      </c>
-      <c r="B59" s="43"/>
+      <c r="A59" s="55" t="s">
+        <v>202</v>
+      </c>
+      <c r="B59" s="49"/>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="B60" s="43" t="s">
-        <v>195</v>
+        <v>203</v>
+      </c>
+      <c r="B60" s="49" t="s">
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -16934,13 +17072,13 @@
       <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="53" width="5.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="56" width="5.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="53" width="5.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="56" width="5.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="21.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="15.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="36.5"/>
@@ -16960,294 +17098,294 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="57" t="s">
+        <v>205</v>
+      </c>
+      <c r="B1" s="57"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="58" t="s">
+        <v>206</v>
+      </c>
+      <c r="E1" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" s="58" t="s">
+        <v>207</v>
+      </c>
+      <c r="G1" s="59"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="60"/>
+      <c r="O1" s="61"/>
+      <c r="P1" s="61"/>
+      <c r="Q1" s="61"/>
+      <c r="R1" s="61"/>
+      <c r="S1" s="61"/>
+      <c r="T1" s="61"/>
+      <c r="U1" s="61"/>
+      <c r="V1" s="61"/>
+      <c r="W1" s="61"/>
+      <c r="X1" s="61"/>
+      <c r="Y1" s="61"/>
+      <c r="Z1" s="61"/>
+      <c r="AA1" s="62"/>
+      <c r="AB1" s="61"/>
+      <c r="AC1" s="61"/>
+      <c r="AD1" s="61"/>
+      <c r="AE1" s="61"/>
+      <c r="AF1" s="61"/>
+      <c r="AG1" s="61"/>
+      <c r="AH1" s="61"/>
+      <c r="AI1" s="61"/>
+      <c r="AJ1" s="61"/>
+      <c r="AK1" s="61"/>
+      <c r="AL1" s="61"/>
+      <c r="AM1" s="61"/>
+      <c r="AN1" s="61"/>
+      <c r="AO1" s="61"/>
+      <c r="AP1" s="61"/>
+      <c r="AQ1" s="61"/>
+      <c r="AR1" s="61"/>
+      <c r="AS1" s="61"/>
+      <c r="AT1" s="63"/>
+    </row>
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="64"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="67" t="s">
+        <v>115</v>
+      </c>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="67"/>
+      <c r="K2" s="67"/>
+      <c r="L2" s="68" t="s">
+        <v>127</v>
+      </c>
+      <c r="M2" s="68"/>
+      <c r="N2" s="68"/>
+      <c r="O2" s="68" t="s">
+        <v>133</v>
+      </c>
+      <c r="P2" s="68"/>
+      <c r="Q2" s="68"/>
+      <c r="R2" s="67" t="s">
+        <v>140</v>
+      </c>
+      <c r="S2" s="67"/>
+      <c r="T2" s="67"/>
+      <c r="U2" s="67"/>
+      <c r="V2" s="67"/>
+      <c r="W2" s="67" t="s">
+        <v>151</v>
+      </c>
+      <c r="X2" s="67"/>
+      <c r="Y2" s="67"/>
+      <c r="Z2" s="67" t="s">
+        <v>158</v>
+      </c>
+      <c r="AA2" s="67"/>
+      <c r="AB2" s="67"/>
+      <c r="AC2" s="67"/>
+      <c r="AD2" s="67"/>
+      <c r="AE2" s="67"/>
+      <c r="AF2" s="67"/>
+      <c r="AG2" s="67"/>
+      <c r="AH2" s="67"/>
+      <c r="AI2" s="67"/>
+      <c r="AJ2" s="67" t="s">
+        <v>179</v>
+      </c>
+      <c r="AK2" s="67"/>
+      <c r="AL2" s="67"/>
+      <c r="AM2" s="67"/>
+      <c r="AN2" s="67"/>
+      <c r="AO2" s="67"/>
+      <c r="AP2" s="67"/>
+      <c r="AQ2" s="67"/>
+      <c r="AR2" s="67"/>
+      <c r="AS2" s="67"/>
+    </row>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="69" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="70" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3" s="40"/>
+      <c r="D3" s="71" t="s">
+        <v>112</v>
+      </c>
+      <c r="E3" s="40"/>
+      <c r="F3" s="71" t="s">
+        <v>116</v>
+      </c>
+      <c r="G3" s="72" t="s">
+        <v>118</v>
+      </c>
+      <c r="H3" s="73" t="s">
+        <v>44</v>
+      </c>
+      <c r="I3" s="73" t="s">
+        <v>121</v>
+      </c>
+      <c r="J3" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="K3" s="74" t="s">
+        <v>125</v>
+      </c>
+      <c r="L3" s="72" t="s">
+        <v>47</v>
+      </c>
+      <c r="M3" s="72" t="s">
+        <v>129</v>
+      </c>
+      <c r="N3" s="74" t="s">
+        <v>131</v>
+      </c>
+      <c r="O3" s="73" t="s">
+        <v>134</v>
+      </c>
+      <c r="P3" s="75" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q3" s="73" t="s">
+        <v>138</v>
+      </c>
+      <c r="R3" s="76" t="s">
+        <v>141</v>
+      </c>
+      <c r="S3" s="73" t="s">
+        <v>143</v>
+      </c>
+      <c r="T3" s="73" t="s">
+        <v>145</v>
+      </c>
+      <c r="U3" s="73" t="s">
+        <v>147</v>
+      </c>
+      <c r="V3" s="74" t="s">
+        <v>149</v>
+      </c>
+      <c r="W3" s="76" t="s">
+        <v>152</v>
+      </c>
+      <c r="X3" s="73" t="s">
+        <v>154</v>
+      </c>
+      <c r="Y3" s="74" t="s">
+        <v>156</v>
+      </c>
+      <c r="Z3" s="76" t="s">
+        <v>159</v>
+      </c>
+      <c r="AA3" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB3" s="72" t="s">
+        <v>163</v>
+      </c>
+      <c r="AC3" s="73" t="s">
+        <v>165</v>
+      </c>
+      <c r="AD3" s="73" t="s">
+        <v>167</v>
+      </c>
+      <c r="AE3" s="73" t="s">
+        <v>169</v>
+      </c>
+      <c r="AF3" s="73" t="s">
+        <v>171</v>
+      </c>
+      <c r="AG3" s="73" t="s">
+        <v>173</v>
+      </c>
+      <c r="AH3" s="73" t="s">
+        <v>175</v>
+      </c>
+      <c r="AI3" s="74" t="s">
+        <v>177</v>
+      </c>
+      <c r="AJ3" s="76" t="s">
+        <v>180</v>
+      </c>
+      <c r="AK3" s="73" t="s">
+        <v>182</v>
+      </c>
+      <c r="AL3" s="73" t="s">
+        <v>184</v>
+      </c>
+      <c r="AM3" s="73" t="s">
+        <v>186</v>
+      </c>
+      <c r="AN3" s="73" t="s">
+        <v>188</v>
+      </c>
+      <c r="AO3" s="73" t="s">
+        <v>190</v>
+      </c>
+      <c r="AP3" s="73" t="s">
+        <v>192</v>
+      </c>
+      <c r="AQ3" s="73" t="s">
+        <v>194</v>
+      </c>
+      <c r="AR3" s="73" t="s">
         <v>196</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="56" t="s">
-        <v>197</v>
-      </c>
-      <c r="E1" s="55" t="s">
+      <c r="AS3" s="74" t="s">
         <v>198</v>
       </c>
-      <c r="F1" s="56" t="s">
-        <v>199</v>
-      </c>
-      <c r="G1" s="57"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
-      <c r="L1" s="58"/>
-      <c r="M1" s="58"/>
-      <c r="N1" s="58"/>
-      <c r="O1" s="59"/>
-      <c r="P1" s="59"/>
-      <c r="Q1" s="59"/>
-      <c r="R1" s="59"/>
-      <c r="S1" s="59"/>
-      <c r="T1" s="59"/>
-      <c r="U1" s="59"/>
-      <c r="V1" s="59"/>
-      <c r="W1" s="59"/>
-      <c r="X1" s="59"/>
-      <c r="Y1" s="59"/>
-      <c r="Z1" s="59"/>
-      <c r="AA1" s="60"/>
-      <c r="AB1" s="59"/>
-      <c r="AC1" s="59"/>
-      <c r="AD1" s="59"/>
-      <c r="AE1" s="59"/>
-      <c r="AF1" s="59"/>
-      <c r="AG1" s="59"/>
-      <c r="AH1" s="59"/>
-      <c r="AI1" s="59"/>
-      <c r="AJ1" s="59"/>
-      <c r="AK1" s="59"/>
-      <c r="AL1" s="59"/>
-      <c r="AM1" s="59"/>
-      <c r="AN1" s="59"/>
-      <c r="AO1" s="59"/>
-      <c r="AP1" s="59"/>
-      <c r="AQ1" s="59"/>
-      <c r="AR1" s="59"/>
-      <c r="AS1" s="59"/>
-      <c r="AT1" s="61"/>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="62"/>
-      <c r="B2" s="63"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="65" t="s">
-        <v>106</v>
-      </c>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="65"/>
-      <c r="K2" s="65"/>
-      <c r="L2" s="66" t="s">
-        <v>118</v>
-      </c>
-      <c r="M2" s="66"/>
-      <c r="N2" s="66"/>
-      <c r="O2" s="66" t="s">
-        <v>124</v>
-      </c>
-      <c r="P2" s="66"/>
-      <c r="Q2" s="66"/>
-      <c r="R2" s="65" t="s">
-        <v>131</v>
-      </c>
-      <c r="S2" s="65"/>
-      <c r="T2" s="65"/>
-      <c r="U2" s="65"/>
-      <c r="V2" s="65"/>
-      <c r="W2" s="65" t="s">
-        <v>142</v>
-      </c>
-      <c r="X2" s="65"/>
-      <c r="Y2" s="65"/>
-      <c r="Z2" s="65" t="s">
-        <v>149</v>
-      </c>
-      <c r="AA2" s="65"/>
-      <c r="AB2" s="65"/>
-      <c r="AC2" s="65"/>
-      <c r="AD2" s="65"/>
-      <c r="AE2" s="65"/>
-      <c r="AF2" s="65"/>
-      <c r="AG2" s="65"/>
-      <c r="AH2" s="65"/>
-      <c r="AI2" s="65"/>
-      <c r="AJ2" s="65" t="s">
-        <v>170</v>
-      </c>
-      <c r="AK2" s="65"/>
-      <c r="AL2" s="65"/>
-      <c r="AM2" s="65"/>
-      <c r="AN2" s="65"/>
-      <c r="AO2" s="65"/>
-      <c r="AP2" s="65"/>
-      <c r="AQ2" s="65"/>
-      <c r="AR2" s="65"/>
-      <c r="AS2" s="65"/>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="67" t="s">
-        <v>65</v>
-      </c>
-      <c r="B3" s="68" t="s">
-        <v>99</v>
-      </c>
-      <c r="C3" s="55"/>
-      <c r="D3" s="69" t="s">
-        <v>103</v>
-      </c>
-      <c r="E3" s="55"/>
-      <c r="F3" s="69" t="s">
-        <v>107</v>
-      </c>
-      <c r="G3" s="70" t="s">
-        <v>109</v>
-      </c>
-      <c r="H3" s="71" t="s">
-        <v>39</v>
-      </c>
-      <c r="I3" s="71" t="s">
-        <v>112</v>
-      </c>
-      <c r="J3" s="71" t="s">
-        <v>114</v>
-      </c>
-      <c r="K3" s="72" t="s">
-        <v>116</v>
-      </c>
-      <c r="L3" s="70" t="s">
-        <v>42</v>
-      </c>
-      <c r="M3" s="70" t="s">
-        <v>120</v>
-      </c>
-      <c r="N3" s="72" t="s">
-        <v>122</v>
-      </c>
-      <c r="O3" s="71" t="s">
-        <v>125</v>
-      </c>
-      <c r="P3" s="73" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q3" s="71" t="s">
-        <v>129</v>
-      </c>
-      <c r="R3" s="74" t="s">
-        <v>132</v>
-      </c>
-      <c r="S3" s="71" t="s">
-        <v>134</v>
-      </c>
-      <c r="T3" s="71" t="s">
-        <v>136</v>
-      </c>
-      <c r="U3" s="71" t="s">
-        <v>138</v>
-      </c>
-      <c r="V3" s="72" t="s">
-        <v>140</v>
-      </c>
-      <c r="W3" s="74" t="s">
-        <v>143</v>
-      </c>
-      <c r="X3" s="71" t="s">
-        <v>145</v>
-      </c>
-      <c r="Y3" s="72" t="s">
-        <v>147</v>
-      </c>
-      <c r="Z3" s="74" t="s">
-        <v>150</v>
-      </c>
-      <c r="AA3" s="75" t="s">
-        <v>152</v>
-      </c>
-      <c r="AB3" s="70" t="s">
-        <v>154</v>
-      </c>
-      <c r="AC3" s="71" t="s">
-        <v>156</v>
-      </c>
-      <c r="AD3" s="71" t="s">
-        <v>158</v>
-      </c>
-      <c r="AE3" s="71" t="s">
-        <v>160</v>
-      </c>
-      <c r="AF3" s="71" t="s">
-        <v>162</v>
-      </c>
-      <c r="AG3" s="71" t="s">
-        <v>164</v>
-      </c>
-      <c r="AH3" s="71" t="s">
-        <v>166</v>
-      </c>
-      <c r="AI3" s="72" t="s">
-        <v>168</v>
-      </c>
-      <c r="AJ3" s="74" t="s">
-        <v>171</v>
-      </c>
-      <c r="AK3" s="71" t="s">
-        <v>173</v>
-      </c>
-      <c r="AL3" s="71" t="s">
-        <v>175</v>
-      </c>
-      <c r="AM3" s="71" t="s">
-        <v>177</v>
-      </c>
-      <c r="AN3" s="71" t="s">
-        <v>179</v>
-      </c>
-      <c r="AO3" s="71" t="s">
-        <v>181</v>
-      </c>
-      <c r="AP3" s="71" t="s">
-        <v>183</v>
-      </c>
-      <c r="AQ3" s="71" t="s">
-        <v>185</v>
-      </c>
-      <c r="AR3" s="71" t="s">
-        <v>187</v>
-      </c>
-      <c r="AS3" s="72" t="s">
-        <v>189</v>
-      </c>
-      <c r="AT3" s="76" t="s">
-        <v>191</v>
+      <c r="AT3" s="78" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="31" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="B4" s="31" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="D4" s="31" t="s">
-        <v>201</v>
-      </c>
-      <c r="M4" s="77"/>
-      <c r="Y4" s="36"/>
+        <v>209</v>
+      </c>
+      <c r="M4" s="79"/>
+      <c r="Y4" s="38"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="31"/>
       <c r="B5" s="31"/>
       <c r="D5" s="31"/>
       <c r="J5" s="1"/>
-      <c r="M5" s="78"/>
+      <c r="M5" s="80"/>
       <c r="P5" s="31"/>
       <c r="Q5" s="1"/>
-      <c r="Y5" s="36"/>
-      <c r="AA5" s="40"/>
+      <c r="Y5" s="38"/>
+      <c r="AA5" s="46"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="31"/>
       <c r="B6" s="31"/>
       <c r="D6" s="31"/>
-      <c r="M6" s="77"/>
-      <c r="Y6" s="36"/>
+      <c r="M6" s="79"/>
+      <c r="Y6" s="38"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="31"/>
       <c r="B7" s="31"/>
       <c r="D7" s="31"/>
-      <c r="M7" s="77"/>
+      <c r="M7" s="79"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="31"/>
@@ -22243,6 +22381,10 @@
     <mergeCell ref="AJ2:AS2"/>
   </mergeCells>
   <dataValidations count="9">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="These sample names must match those provided in the VCF file(s)" promptTitle="Metadata and VCF" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E1 B5:B1003" type="none">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Must match an analysis alias provided in the &quot;ANALYSIS&quot; sheet&#10;Multiple entries can be separated with a comma&#10;e.g. analysis1,analysis2" promptTitle="Analysis alias" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A3" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
@@ -22260,10 +22402,6 @@
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="These sample names must match those provided in the VCF file(s). They can be different from the sample name provided to new BioSamples  " promptTitle="Sample Name in VCF" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B3" type="none">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="These sample names must match those provided in the VCF file(s)" promptTitle="Metadata and VCF" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E1 B5:B1003" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -22301,7 +22439,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="153.83"/>
@@ -22316,19 +22454,19 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="33" t="s">
-        <v>65</v>
+      <c r="A2" s="35" t="s">
+        <v>74</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="33" t="s">
-        <v>203</v>
+      <c r="A3" s="35" t="s">
+        <v>211</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>

</xml_diff>